<commit_message>
Supernova in one pass
</commit_message>
<xml_diff>
--- a/ArrayFromPycharm.xlsx
+++ b/ArrayFromPycharm.xlsx
@@ -406,13 +406,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -502,13 +502,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -598,10 +598,10 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>

</xml_diff>

<commit_message>
for Johnnik 2021.01.31 Supernova in one pass+Clusters showЖенечка
</commit_message>
<xml_diff>
--- a/ArrayFromPycharm.xlsx
+++ b/ArrayFromPycharm.xlsx
@@ -403,13 +403,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -432,10 +432,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -461,13 +461,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -499,13 +499,13 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -528,10 +528,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -557,13 +557,13 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -624,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>